<commit_message>
Priyanka kale added bulk upload
</commit_message>
<xml_diff>
--- a/admin/public/products.xlsx
+++ b/admin/public/products.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="121">
   <si>
     <t xml:space="preserve">section</t>
   </si>
@@ -53,13 +53,13 @@
     <t xml:space="preserve">currency</t>
   </si>
   <si>
-    <t xml:space="preserve">actualPrice</t>
+    <t xml:space="preserve">originalPrice</t>
   </si>
   <si>
     <t xml:space="preserve">discountPercent</t>
   </si>
   <si>
-    <t xml:space="preserve">offeredPrice</t>
+    <t xml:space="preserve">discountedPrice</t>
   </si>
   <si>
     <t xml:space="preserve">availableQuantity</t>
@@ -101,7 +101,7 @@
     <t xml:space="preserve">color</t>
   </si>
   <si>
-    <t xml:space="preserve">Main-Site</t>
+    <t xml:space="preserve">tags</t>
   </si>
   <si>
     <t xml:space="preserve">Electronics</t>
@@ -152,6 +152,9 @@
     <t xml:space="preserve">#333</t>
   </si>
   <si>
+    <t xml:space="preserve">hashtag1,hashrag2</t>
+  </si>
+  <si>
     <t xml:space="preserve">AB002</t>
   </si>
   <si>
@@ -209,6 +212,9 @@
     <t xml:space="preserve">#999</t>
   </si>
   <si>
+    <t xml:space="preserve">Fashion</t>
+  </si>
+  <si>
     <t xml:space="preserve">Baby &amp; Kids</t>
   </si>
   <si>
@@ -339,6 +345,45 @@
   </si>
   <si>
     <t xml:space="preserve">L</t>
+  </si>
+  <si>
+    <t xml:space="preserve">subcategory</t>
+  </si>
+  <si>
+    <t xml:space="preserve">role based login</t>
+  </si>
+  <si>
+    <t xml:space="preserve">update shopping cart, continue shopping -remove</t>
+  </si>
+  <si>
+    <t xml:space="preserve">quick view – consize</t>
+  </si>
+  <si>
+    <t xml:space="preserve">On hover- show cart </t>
+  </si>
+  <si>
+    <t xml:space="preserve">onclick goto cart</t>
+  </si>
+  <si>
+    <t xml:space="preserve">gift wrap – remove</t>
+  </si>
+  <si>
+    <t xml:space="preserve">comment -remove</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0 shipping charges = free</t>
+  </si>
+  <si>
+    <t xml:space="preserve">discount coupon </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Swal – remove</t>
+  </si>
+  <si>
+    <t xml:space="preserve">my order - </t>
+  </si>
+  <si>
+    <t xml:space="preserve">feedback after delivered &amp; paid</t>
   </si>
 </sst>
 </file>
@@ -736,8 +781,8 @@
   </sheetPr>
   <dimension ref="A1:AMJ6"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="R1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="AB2" activeCellId="0" sqref="AB2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -753,7 +798,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="10.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="13.28"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="15.99"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="12.25"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="15.34"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="18.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="18.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="0" width="18.71"/>
@@ -845,19 +890,20 @@
       <c r="Z1" s="2" t="s">
         <v>25</v>
       </c>
+      <c r="AA1" s="2" t="s">
+        <v>26</v>
+      </c>
       <c r="AMI1" s="0"/>
       <c r="AMJ1" s="0"/>
     </row>
-    <row r="2" customFormat="false" ht="108.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="123.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="3" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="C2" s="3" t="s">
         <v>28</v>
       </c>
+      <c r="C2" s="3"/>
       <c r="D2" s="3" t="s">
         <v>29</v>
       </c>
@@ -922,34 +968,35 @@
       <c r="Z2" s="0" t="s">
         <v>42</v>
       </c>
+      <c r="AA2" s="3" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="3" customFormat="false" ht="105.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="C3" s="3" t="s">
         <v>28</v>
       </c>
+      <c r="C3" s="3"/>
       <c r="D3" s="3" t="s">
         <v>29</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="H3" s="3" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="I3" s="3" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="J3" s="3" t="s">
         <v>35</v>
@@ -983,48 +1030,46 @@
         <v>37</v>
       </c>
       <c r="V3" s="3" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="W3" s="3" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="X3" s="3" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="Y3" s="6" t="s">
         <v>41</v>
       </c>
       <c r="Z3" s="0" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="87.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="3" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="C4" s="3" t="s">
         <v>28</v>
       </c>
+      <c r="C4" s="3"/>
       <c r="D4" s="3" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="H4" s="3" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="I4" s="3" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="J4" s="3" t="s">
         <v>35</v>
@@ -1058,48 +1103,48 @@
         <v>37</v>
       </c>
       <c r="V4" s="3" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="W4" s="3" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="X4" s="3" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="Y4" s="6" t="s">
         <v>41</v>
       </c>
       <c r="Z4" s="0" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="69.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>26</v>
+        <v>63</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="G5" s="3" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="H5" s="3" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="I5" s="0" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="J5" s="0" t="s">
         <v>35</v>
@@ -1120,33 +1165,33 @@
         <v>37</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="69.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>26</v>
+        <v>63</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="G6" s="6" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="H6" s="3" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="I6" s="3" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="J6" s="0" t="s">
         <v>35</v>
@@ -1179,29 +1224,25 @@
         <v>37</v>
       </c>
       <c r="V6" s="3" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="W6" s="0" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="X6" s="0" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="Y6" s="6" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="Z6" s="0" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
     </row>
   </sheetData>
-  <dataValidations count="5">
+  <dataValidations count="4">
     <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="Q1:Q6" type="list">
       <formula1>"Draft,Publish,Unpublish"</formula1>
-      <formula2>0</formula2>
-    </dataValidation>
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="A2:A4" type="list">
-      <formula1>"Main-Site,Grocery"</formula1>
       <formula2>0</formula2>
     </dataValidation>
     <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="J2:J4" type="list">
@@ -1232,10 +1273,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A2:O23"/>
+  <dimension ref="A2:O41"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A5" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="I42" activeCellId="0" sqref="I42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1249,54 +1290,54 @@
   <sheetData>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="F2" s="0" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="G2" s="0" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="H2" s="0" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="I2" s="0" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="J2" s="0" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="K2" s="0" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="L2" s="0" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="M2" s="0" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="N2" s="0" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="O2" s="0" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E3" s="0" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="F3" s="0" t="n">
         <v>15</v>
@@ -1311,125 +1352,198 @@
         <v>75</v>
       </c>
       <c r="J3" s="0" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="K3" s="0" t="n">
         <v>10</v>
       </c>
       <c r="L3" s="0" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F4" s="0" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F5" s="0" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F6" s="0" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F7" s="0" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C8" s="0" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C9" s="0" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C10" s="0" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C11" s="0" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="D11" s="0" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C12" s="0" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="D12" s="0" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C13" s="0" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="D13" s="0" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C14" s="0" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="D14" s="0" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C15" s="0" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C16" s="0" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C17" s="0" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C18" s="0" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C19" s="0" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C20" s="0" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C21" s="0" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C22" s="0" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C23" s="0" t="s">
-        <v>102</v>
+        <v>104</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H28" s="0" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H29" s="0" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H30" s="0" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H31" s="0" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H32" s="0" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H33" s="0" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H34" s="0" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H35" s="0" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H36" s="0" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H37" s="0" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H38" s="0" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H39" s="0" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H40" s="0" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H41" s="0" t="s">
+        <v>119</v>
+      </c>
+      <c r="I41" s="0" t="s">
+        <v>120</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
priyanka k added return product functionality
</commit_message>
<xml_diff>
--- a/admin/public/products.xlsx
+++ b/admin/public/products.xlsx
@@ -21,7 +21,10 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="124">
+  <si>
+    <t xml:space="preserve">vendorID</t>
+  </si>
   <si>
     <t xml:space="preserve">section</t>
   </si>
@@ -116,7 +119,7 @@
     <t xml:space="preserve">AB001</t>
   </si>
   <si>
-    <t xml:space="preserve">AB001A</t>
+    <t xml:space="preserve">AB001-1</t>
   </si>
   <si>
     <t xml:space="preserve">Redmi Note 7S</t>
@@ -158,7 +161,7 @@
     <t xml:space="preserve">AB002</t>
   </si>
   <si>
-    <t xml:space="preserve">AB002A</t>
+    <t xml:space="preserve">AB002-1</t>
   </si>
   <si>
     <t xml:space="preserve">Redmi Y3</t>
@@ -188,7 +191,7 @@
     <t xml:space="preserve">AB003</t>
   </si>
   <si>
-    <t xml:space="preserve">AB003A</t>
+    <t xml:space="preserve">AB003-1</t>
   </si>
   <si>
     <t xml:space="preserve">Realme 3 Pro (Nitro Blue, 4GB RAM, 64GB Storage)</t>
@@ -227,7 +230,7 @@
     <t xml:space="preserve">AB004</t>
   </si>
   <si>
-    <t xml:space="preserve">AB004A</t>
+    <t xml:space="preserve">AB004-1</t>
   </si>
   <si>
     <t xml:space="preserve">Boys Festive</t>
@@ -239,6 +242,24 @@
     <t xml:space="preserve">💡Tip:For the best fit, buy one size smaller than your usual size.</t>
   </si>
   <si>
+    <t xml:space="preserve">Special PriceGet extra 8% off (price inclusive of discount)T&amp;C</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bank Offer 10% Instant Discount on ICICI Bank Credit and Debit CardsT&amp;C</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bank Offer 5% Unlimited Cashback on Flipkart Axis Bank Credit CardT&amp;C</t>
+  </si>
+  <si>
+    <t xml:space="preserve">large</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AB004-2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">medium</t>
+  </si>
+  <si>
     <t xml:space="preserve">Girl’s Clothing</t>
   </si>
   <si>
@@ -248,7 +269,7 @@
     <t xml:space="preserve">AB005</t>
   </si>
   <si>
-    <t xml:space="preserve">AB005A</t>
+    <t xml:space="preserve">AB005-1</t>
   </si>
   <si>
     <t xml:space="preserve">Girls Maxi Full Length Party Dress</t>
@@ -258,18 +279,6 @@
   </si>
   <si>
     <t xml:space="preserve">Tip:For the best fit, buy one size smaller than your usual size.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Special PriceGet extra 8% off (price inclusive of discount)T&amp;C</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Bank Offer 10% Instant Discount on ICICI Bank Credit and Debit CardsT&amp;C</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Bank Offer 5% Unlimited Cashback on Flipkart Axis Bank Credit CardT&amp;C</t>
-  </si>
-  <si>
-    <t xml:space="preserve">medium</t>
   </si>
   <si>
     <t xml:space="preserve">#ec47cd</t>
@@ -390,17 +399,19 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="3">
+  <numFmts count="4">
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="#,##0"/>
-    <numFmt numFmtId="166" formatCode="0.00%"/>
+    <numFmt numFmtId="166" formatCode="&quot;TRUE&quot;;&quot;TRUE&quot;;&quot;FALSE&quot;"/>
+    <numFmt numFmtId="167" formatCode="0.00%"/>
   </numFmts>
-  <fonts count="17">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -419,140 +430,22 @@
     </font>
     <font>
       <b val="true"/>
-      <sz val="24"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="18"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF333333"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <i val="true"/>
-      <sz val="10"/>
-      <color rgb="FF808080"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <u val="single"/>
-      <sz val="10"/>
-      <color rgb="FF0000EE"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF006600"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF996600"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FFCC0000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b val="true"/>
-      <sz val="10"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b val="true"/>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b val="true"/>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor rgb="FFFFFFFF"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFCCFFCC"/>
-        <bgColor rgb="FFCCFFFF"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCCCC"/>
-        <bgColor rgb="FFDDDDDD"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFCC0000"/>
-        <bgColor rgb="FF800000"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF000000"/>
-        <bgColor rgb="FF003300"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF808080"/>
-        <bgColor rgb="FF969696"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFDDDDDD"/>
-        <bgColor rgb="FFFFCCCC"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="2">
+  <borders count="1">
     <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
@@ -560,23 +453,8 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left style="thin">
-        <color rgb="FF808080"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF808080"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF808080"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF808080"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
-  <cellStyleXfs count="37">
+  <cellStyleXfs count="20">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -600,69 +478,18 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="2" borderId="1" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="10" fillId="3" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="11" fillId="2" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="12" fillId="4" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="13" fillId="5" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="14" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="15" fillId="6" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="15" fillId="7" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="14" fillId="8" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
   </cellStyleXfs>
   <cellXfs count="8">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
@@ -673,7 +500,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -681,96 +508,19 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
-  <cellStyles count="23">
+  <cellStyles count="6">
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
     <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
     <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
     <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
     <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
     <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
-    <cellStyle name="Heading" xfId="20" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Heading 1" xfId="21" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Heading 2" xfId="22" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Text" xfId="23" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Note" xfId="24" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Footnote" xfId="25" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Hyperlink" xfId="26" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Status" xfId="27" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Good" xfId="28" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Neutral" xfId="29" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Bad" xfId="30" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Warning" xfId="31" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Error" xfId="32" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Accent" xfId="33" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Accent 1" xfId="34" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Accent 2" xfId="35" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Accent 3" xfId="36" builtinId="53" customBuiltin="true"/>
   </cellStyles>
-  <colors>
-    <indexedColors>
-      <rgbColor rgb="FF000000"/>
-      <rgbColor rgb="FFFFFFFF"/>
-      <rgbColor rgb="FFCC0000"/>
-      <rgbColor rgb="FF00FF00"/>
-      <rgbColor rgb="FF0000EE"/>
-      <rgbColor rgb="FFFFFF00"/>
-      <rgbColor rgb="FFFF00FF"/>
-      <rgbColor rgb="FF00FFFF"/>
-      <rgbColor rgb="FF800000"/>
-      <rgbColor rgb="FF006600"/>
-      <rgbColor rgb="FF000080"/>
-      <rgbColor rgb="FF996600"/>
-      <rgbColor rgb="FF800080"/>
-      <rgbColor rgb="FF008080"/>
-      <rgbColor rgb="FFC0C0C0"/>
-      <rgbColor rgb="FF808080"/>
-      <rgbColor rgb="FF9999FF"/>
-      <rgbColor rgb="FF993366"/>
-      <rgbColor rgb="FFFFFFCC"/>
-      <rgbColor rgb="FFCCFFFF"/>
-      <rgbColor rgb="FF660066"/>
-      <rgbColor rgb="FFFF8080"/>
-      <rgbColor rgb="FF0066CC"/>
-      <rgbColor rgb="FFDDDDDD"/>
-      <rgbColor rgb="FF000080"/>
-      <rgbColor rgb="FFFF00FF"/>
-      <rgbColor rgb="FFFFFF00"/>
-      <rgbColor rgb="FF00FFFF"/>
-      <rgbColor rgb="FF800080"/>
-      <rgbColor rgb="FF800000"/>
-      <rgbColor rgb="FF008080"/>
-      <rgbColor rgb="FF0000FF"/>
-      <rgbColor rgb="FF00CCFF"/>
-      <rgbColor rgb="FFCCFFFF"/>
-      <rgbColor rgb="FFCCFFCC"/>
-      <rgbColor rgb="FFFFFF99"/>
-      <rgbColor rgb="FF99CCFF"/>
-      <rgbColor rgb="FFFF99CC"/>
-      <rgbColor rgb="FFCC99FF"/>
-      <rgbColor rgb="FFFFCCCC"/>
-      <rgbColor rgb="FF3366FF"/>
-      <rgbColor rgb="FF33CCCC"/>
-      <rgbColor rgb="FF99CC00"/>
-      <rgbColor rgb="FFFFCC00"/>
-      <rgbColor rgb="FFFF9900"/>
-      <rgbColor rgb="FFFF6600"/>
-      <rgbColor rgb="FF666699"/>
-      <rgbColor rgb="FF969696"/>
-      <rgbColor rgb="FF003366"/>
-      <rgbColor rgb="FF339966"/>
-      <rgbColor rgb="FF003300"/>
-      <rgbColor rgb="FF333300"/>
-      <rgbColor rgb="FF993300"/>
-      <rgbColor rgb="FF993366"/>
-      <rgbColor rgb="FF333399"/>
-      <rgbColor rgb="FF333333"/>
-    </indexedColors>
-  </colors>
 </styleSheet>
 </file>
 
@@ -779,134 +529,136 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AMJ6"/>
+  <dimension ref="A1:AMJ7"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="R1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="AB2" activeCellId="0" sqref="AB2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="I1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="N2" activeCellId="0" sqref="N2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="20"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="16.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="19.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="14.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="6" style="0" width="23"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="56.72"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="21.28"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="10.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="13.28"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="15.99"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="15.34"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="18.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="18.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="0" width="18.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="0" width="9.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="18" style="0" width="8.53"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="0" width="15.08"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="0" width="16.28"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="23" min="22" style="0" width="23.72"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="24" min="24" style="0" width="20.22"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="25" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="20"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="16.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="19.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="14.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="7" style="0" width="23"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="56.72"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="21.28"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="10.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="13.28"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="13" style="0" width="15.99"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="18.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="0" width="20.94"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="0" width="18.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="0" width="9.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="0" width="10.88"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="0" width="13.37"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="0" width="15.08"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="22" style="0" width="16.28"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="24" min="23" style="0" width="23.72"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="25" min="25" style="0" width="20.22"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="26" style="0" width="8.53"/>
   </cols>
   <sheetData>
-    <row r="1" s="2" customFormat="true" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" s="1" customFormat="true" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="I1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="J1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="K1" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="L1" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="M1" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="N1" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="O1" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="P1" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="Q1" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="R1" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="S1" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="T1" s="1" t="s">
+      <c r="T1" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="U1" s="1" t="s">
+      <c r="U1" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="V1" s="1" t="s">
+      <c r="V1" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="W1" s="1" t="s">
+      <c r="W1" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="X1" s="1" t="s">
+      <c r="X1" s="2" t="s">
         <v>23</v>
       </c>
       <c r="Y1" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="Z1" s="2" t="s">
+      <c r="Z1" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="AA1" s="2" t="s">
+      <c r="AA1" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="AMI1" s="0"/>
+      <c r="AB1" s="1" t="s">
+        <v>27</v>
+      </c>
       <c r="AMJ1" s="0"/>
     </row>
     <row r="2" customFormat="false" ht="123.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="3" t="s">
-        <v>27</v>
+      <c r="A2" s="0" t="n">
+        <v>101</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="C2" s="3"/>
-      <c r="D2" s="3" t="s">
+      <c r="C2" s="3" t="s">
         <v>29</v>
       </c>
+      <c r="D2" s="3"/>
       <c r="E2" s="3" t="s">
         <v>30</v>
       </c>
@@ -925,33 +677,34 @@
       <c r="J2" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="K2" s="4" t="n">
+      <c r="K2" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="L2" s="4" t="n">
         <v>9999</v>
       </c>
-      <c r="L2" s="4"/>
-      <c r="M2" s="5"/>
+      <c r="M2" s="4" t="n">
+        <v>20</v>
+      </c>
       <c r="N2" s="3" t="n">
+        <v>8000</v>
+      </c>
+      <c r="O2" s="3" t="n">
         <v>4</v>
       </c>
-      <c r="O2" s="3"/>
       <c r="P2" s="3"/>
-      <c r="Q2" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="R2" s="5" t="n">
-        <f aca="false">TRUE()</f>
+      <c r="Q2" s="3"/>
+      <c r="R2" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="S2" s="5" t="b">
         <v>1</v>
       </c>
-      <c r="S2" s="5" t="n">
-        <f aca="false">TRUE()</f>
+      <c r="T2" s="5" t="b">
         <v>1</v>
       </c>
-      <c r="T2" s="5" t="n">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="U2" s="3" t="s">
-        <v>37</v>
+      <c r="U2" s="5" t="b">
+        <v>1</v>
       </c>
       <c r="V2" s="3" t="s">
         <v>38</v>
@@ -962,29 +715,32 @@
       <c r="X2" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="Y2" s="6" t="s">
+      <c r="Y2" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="Z2" s="0" t="s">
+      <c r="Z2" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="AA2" s="3" t="s">
+      <c r="AA2" s="0" t="s">
         <v>43</v>
       </c>
+      <c r="AB2" s="3" t="s">
+        <v>44</v>
+      </c>
     </row>
     <row r="3" customFormat="false" ht="105.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="3" t="s">
-        <v>27</v>
+      <c r="A3" s="0" t="n">
+        <v>101</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="C3" s="3"/>
-      <c r="D3" s="3" t="s">
+      <c r="C3" s="3" t="s">
         <v>29</v>
       </c>
+      <c r="D3" s="3"/>
       <c r="E3" s="3" t="s">
-        <v>44</v>
+        <v>30</v>
       </c>
       <c r="F3" s="3" t="s">
         <v>45</v>
@@ -999,38 +755,39 @@
         <v>48</v>
       </c>
       <c r="J3" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="K3" s="3" t="n">
+        <v>49</v>
+      </c>
+      <c r="K3" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="L3" s="3" t="n">
         <v>8999</v>
       </c>
-      <c r="L3" s="3"/>
-      <c r="M3" s="5"/>
+      <c r="M3" s="3" t="n">
+        <v>10</v>
+      </c>
       <c r="N3" s="3" t="n">
+        <v>8910</v>
+      </c>
+      <c r="O3" s="3" t="n">
         <v>4</v>
       </c>
-      <c r="O3" s="3"/>
       <c r="P3" s="3"/>
-      <c r="Q3" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="R3" s="5" t="n">
-        <f aca="false">TRUE()</f>
+      <c r="Q3" s="3"/>
+      <c r="R3" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="S3" s="5" t="b">
         <v>1</v>
       </c>
-      <c r="S3" s="5" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="T3" s="5" t="n">
-        <f aca="false">FALSE()</f>
+      <c r="T3" s="5" t="b">
         <v>0</v>
       </c>
-      <c r="U3" s="3" t="s">
-        <v>37</v>
+      <c r="U3" s="5" t="b">
+        <v>0</v>
       </c>
       <c r="V3" s="3" t="s">
-        <v>49</v>
+        <v>38</v>
       </c>
       <c r="W3" s="3" t="s">
         <v>50</v>
@@ -1038,24 +795,27 @@
       <c r="X3" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="Y3" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="Z3" s="0" t="s">
+      <c r="Y3" s="3" t="s">
         <v>52</v>
       </c>
+      <c r="Z3" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="AA3" s="0" t="s">
+        <v>53</v>
+      </c>
     </row>
     <row r="4" customFormat="false" ht="87.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A4" s="3" t="s">
-        <v>27</v>
+      <c r="A4" s="0" t="n">
+        <v>101</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="C4" s="3"/>
-      <c r="D4" s="3" t="s">
-        <v>53</v>
-      </c>
+      <c r="C4" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="D4" s="3"/>
       <c r="E4" s="3" t="s">
         <v>54</v>
       </c>
@@ -1072,38 +832,39 @@
         <v>58</v>
       </c>
       <c r="J4" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="K4" s="3" t="n">
+        <v>59</v>
+      </c>
+      <c r="K4" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="L4" s="3" t="n">
         <v>12999</v>
       </c>
-      <c r="L4" s="3"/>
-      <c r="M4" s="5"/>
+      <c r="M4" s="3" t="n">
+        <v>10</v>
+      </c>
       <c r="N4" s="3" t="n">
+        <v>12997</v>
+      </c>
+      <c r="O4" s="3" t="n">
         <v>4</v>
       </c>
-      <c r="O4" s="3"/>
       <c r="P4" s="3"/>
-      <c r="Q4" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="R4" s="5" t="n">
-        <f aca="false">TRUE()</f>
+      <c r="Q4" s="3"/>
+      <c r="R4" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="S4" s="5" t="b">
         <v>1</v>
       </c>
-      <c r="S4" s="5" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="T4" s="5" t="n">
-        <f aca="false">FALSE()</f>
+      <c r="T4" s="5" t="b">
         <v>0</v>
       </c>
-      <c r="U4" s="3" t="s">
-        <v>37</v>
+      <c r="U4" s="5" t="b">
+        <v>0</v>
       </c>
       <c r="V4" s="3" t="s">
-        <v>59</v>
+        <v>38</v>
       </c>
       <c r="W4" s="3" t="s">
         <v>60</v>
@@ -1111,27 +872,30 @@
       <c r="X4" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="Y4" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="Z4" s="0" t="s">
+      <c r="Y4" s="3" t="s">
         <v>62</v>
       </c>
+      <c r="Z4" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="AA4" s="0" t="s">
+        <v>63</v>
+      </c>
     </row>
     <row r="5" customFormat="false" ht="69.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
-        <v>63</v>
-      </c>
-      <c r="B5" s="3" t="s">
+      <c r="A5" s="0" t="n">
+        <v>101</v>
+      </c>
+      <c r="B5" s="0" t="s">
         <v>64</v>
       </c>
-      <c r="C5" s="0" t="s">
+      <c r="C5" s="3" t="s">
         <v>65</v>
       </c>
       <c r="D5" s="0" t="s">
         <v>66</v>
       </c>
-      <c r="E5" s="3" t="s">
+      <c r="E5" s="0" t="s">
         <v>67</v>
       </c>
       <c r="F5" s="3" t="s">
@@ -1143,117 +907,225 @@
       <c r="H5" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="I5" s="0" t="s">
+      <c r="I5" s="3" t="s">
         <v>71</v>
       </c>
       <c r="J5" s="0" t="s">
-        <v>35</v>
-      </c>
-      <c r="K5" s="0" t="n">
+        <v>72</v>
+      </c>
+      <c r="K5" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="L5" s="0" t="n">
         <v>899</v>
       </c>
-      <c r="L5" s="7" t="n">
-        <v>0.2</v>
-      </c>
-      <c r="M5" s="0" t="n">
-        <v>699</v>
-      </c>
-      <c r="Q5" s="3" t="s">
+      <c r="M5" s="3" t="n">
+        <v>5</v>
+      </c>
+      <c r="N5" s="3" t="n">
+        <v>855</v>
+      </c>
+      <c r="O5" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="R5" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="S5" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="T5" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="U5" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="V5" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="W5" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="X5" s="0" t="s">
+        <v>74</v>
+      </c>
+      <c r="Y5" s="0" t="s">
+        <v>75</v>
+      </c>
+      <c r="Z5" s="0" t="s">
+        <v>76</v>
+      </c>
+      <c r="AA5" s="0" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="69.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="n">
+        <v>101</v>
+      </c>
+      <c r="B6" s="0" t="s">
+        <v>64</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="D6" s="0" t="s">
+        <v>66</v>
+      </c>
+      <c r="E6" s="0" t="s">
+        <v>67</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="G6" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="H6" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="I6" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="J6" s="0" t="s">
+        <v>72</v>
+      </c>
+      <c r="K6" s="0" t="s">
         <v>36</v>
       </c>
-      <c r="U5" s="3" t="s">
+      <c r="L6" s="0" t="n">
+        <v>899</v>
+      </c>
+      <c r="M6" s="3" t="n">
+        <v>5</v>
+      </c>
+      <c r="N6" s="3" t="n">
+        <v>855</v>
+      </c>
+      <c r="O6" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="R6" s="3" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="6" customFormat="false" ht="69.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="s">
-        <v>63</v>
-      </c>
-      <c r="B6" s="3" t="s">
+      <c r="S6" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="T6" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="U6" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="V6" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="W6" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="X6" s="0" t="s">
+        <v>74</v>
+      </c>
+      <c r="Y6" s="0" t="s">
+        <v>75</v>
+      </c>
+      <c r="Z6" s="0" t="s">
+        <v>78</v>
+      </c>
+      <c r="AA6" s="0" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="69.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="n">
+        <v>101</v>
+      </c>
+      <c r="B7" s="0" t="s">
         <v>64</v>
       </c>
-      <c r="C6" s="6" t="s">
-        <v>72</v>
-      </c>
-      <c r="D6" s="0" t="s">
+      <c r="C7" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="D7" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="E7" s="0" t="s">
+        <v>80</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="G7" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="H7" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="I7" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="J7" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="K7" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="L7" s="0" t="n">
+        <v>1199</v>
+      </c>
+      <c r="M7" s="3" t="n">
+        <v>5</v>
+      </c>
+      <c r="N7" s="3"/>
+      <c r="O7" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="R7" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="S7" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="T7" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="U7" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="V7" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="W7" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="E6" s="3" t="s">
+      <c r="X7" s="0" t="s">
         <v>74</v>
       </c>
-      <c r="F6" s="3" t="s">
+      <c r="Y7" s="0" t="s">
         <v>75</v>
       </c>
-      <c r="G6" s="6" t="s">
-        <v>76</v>
-      </c>
-      <c r="H6" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="I6" s="3" t="s">
+      <c r="Z7" s="6" t="s">
         <v>78</v>
       </c>
-      <c r="J6" s="0" t="s">
-        <v>35</v>
-      </c>
-      <c r="K6" s="0" t="n">
-        <v>1199</v>
-      </c>
-      <c r="L6" s="7" t="n">
-        <v>0.1</v>
-      </c>
-      <c r="M6" s="0" t="n">
-        <v>1000</v>
-      </c>
-      <c r="N6" s="0" t="n">
-        <v>4</v>
-      </c>
-      <c r="Q6" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="R6" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="S6" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="T6" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="U6" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="V6" s="3" t="s">
-        <v>79</v>
-      </c>
-      <c r="W6" s="0" t="s">
-        <v>80</v>
-      </c>
-      <c r="X6" s="0" t="s">
-        <v>81</v>
-      </c>
-      <c r="Y6" s="6" t="s">
-        <v>82</v>
-      </c>
-      <c r="Z6" s="0" t="s">
-        <v>83</v>
+      <c r="AA7" s="0" t="s">
+        <v>86</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="4">
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="Q1:Q6" type="list">
+    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="R1:R7" type="list">
       <formula1>"Draft,Publish,Unpublish"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="J2:J4" type="list">
+    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="K2:K4" type="list">
       <formula1>"inr,usd,eur,gbp"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="M2:M4 R2:T4" type="list">
+    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="S2:U7" type="list">
       <formula1>"true,false"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="U2:U6" type="list">
+    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="V2:V7" type="list">
       <formula1>"Single,Dozen,Kilograms,Miligrams,Liters,Mililiters"</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -1290,54 +1162,54 @@
   <sheetData>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>87</v>
+        <v>90</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="F2" s="0" t="s">
-        <v>89</v>
+        <v>92</v>
       </c>
       <c r="G2" s="0" t="s">
-        <v>90</v>
+        <v>93</v>
       </c>
       <c r="H2" s="0" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
       <c r="I2" s="0" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="J2" s="0" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="K2" s="0" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="L2" s="0" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
       <c r="M2" s="0" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
       <c r="N2" s="0" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="O2" s="0" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E3" s="0" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="F3" s="0" t="n">
         <v>15</v>
@@ -1352,198 +1224,198 @@
         <v>75</v>
       </c>
       <c r="J3" s="0" t="s">
-        <v>100</v>
+        <v>103</v>
       </c>
       <c r="K3" s="0" t="n">
         <v>10</v>
       </c>
       <c r="L3" s="0" t="s">
-        <v>101</v>
+        <v>104</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F4" s="0" t="s">
-        <v>102</v>
+        <v>105</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F5" s="0" t="s">
-        <v>103</v>
+        <v>106</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F6" s="0" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F7" s="0" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C8" s="0" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C9" s="0" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C10" s="0" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C11" s="0" t="s">
-        <v>106</v>
+        <v>109</v>
       </c>
       <c r="D11" s="0" t="s">
-        <v>107</v>
+        <v>110</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C12" s="0" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="D12" s="0" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C13" s="0" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="D13" s="0" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C14" s="0" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
       <c r="D14" s="0" t="s">
-        <v>106</v>
+        <v>109</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C15" s="0" t="s">
-        <v>107</v>
+        <v>110</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C16" s="0" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C17" s="0" t="s">
-        <v>107</v>
+        <v>110</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C18" s="0" t="s">
-        <v>107</v>
+        <v>110</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C19" s="0" t="s">
-        <v>107</v>
+        <v>110</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C20" s="0" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C21" s="0" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C22" s="0" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C23" s="0" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H28" s="0" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H29" s="0" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H30" s="0" t="s">
-        <v>108</v>
+        <v>111</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H31" s="0" t="s">
-        <v>109</v>
+        <v>112</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H32" s="0" t="s">
-        <v>110</v>
+        <v>113</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H33" s="0" t="s">
-        <v>111</v>
+        <v>114</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H34" s="0" t="s">
-        <v>112</v>
+        <v>115</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H35" s="0" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H36" s="0" t="s">
-        <v>114</v>
+        <v>117</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H37" s="0" t="s">
-        <v>115</v>
+        <v>118</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H38" s="0" t="s">
-        <v>116</v>
+        <v>119</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H39" s="0" t="s">
-        <v>117</v>
+        <v>120</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H40" s="0" t="s">
-        <v>118</v>
+        <v>121</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H41" s="0" t="s">
-        <v>119</v>
+        <v>122</v>
       </c>
       <c r="I41" s="0" t="s">
-        <v>120</v>
+        <v>123</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Priyanka kale solved issues in bulk upload
</commit_message>
<xml_diff>
--- a/admin/public/products.xlsx
+++ b/admin/public/products.xlsx
@@ -239,7 +239,7 @@
     <t xml:space="preserve">Brand : Digimart Style Code : DEZINE BLACK AND PINK KOLI Brand Color : BLACK Size : 7 - 8 Years Type : Maxi Dress Occasion : Party Ideal For : Boys Pattern : Applique Primary Color : Black Fabric : Polycotton Sleeve Type : 3/4 Sleeve Suitable For : Western Wear Fabric Details : Polycotton,Lycra Generic Name : Kids Dress</t>
   </si>
   <si>
-    <t xml:space="preserve">💡Tip:For the best fit, buy one size smaller than your usual size.</t>
+    <t xml:space="preserve">Tip:For the best fit, buy one size smaller than your usual size.</t>
   </si>
   <si>
     <t xml:space="preserve">Special PriceGet extra 8% off (price inclusive of discount)T&amp;C</t>
@@ -260,6 +260,9 @@
     <t xml:space="preserve">medium</t>
   </si>
   <si>
+    <t xml:space="preserve">FASHION</t>
+  </si>
+  <si>
     <t xml:space="preserve">Girl’s Clothing</t>
   </si>
   <si>
@@ -276,9 +279,6 @@
   </si>
   <si>
     <t xml:space="preserve">Brand : KAARIGARI Style Code : DEZINE BLACK AND PINK KOLI Brand Color : BLACK Size : 7 - 8 Years Type : Maxi Dress Occasion : Party Ideal For : Girls Pattern : Applique Primary Color : Black Fabric : Polycotton Sleeve Type : 3/4 Sleeve Suitable For : Western Wear Fabric Details : Polycotton,Lycra Generic Name : Kids Dress</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Tip:For the best fit, buy one size smaller than your usual size.</t>
   </si>
   <si>
     <t xml:space="preserve">#ec47cd</t>
@@ -531,8 +531,8 @@
   </sheetPr>
   <dimension ref="A1:AMJ7"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="I1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="N2" activeCellId="0" sqref="N2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="J3" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="N7" activeCellId="0" sqref="N7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1036,36 +1036,36 @@
         <v>43</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="69.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="n">
         <v>101</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>64</v>
+        <v>79</v>
       </c>
       <c r="C7" s="3" t="s">
         <v>65</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="E7" s="0" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="G7" s="3" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="H7" s="6" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="I7" s="3" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="J7" s="3" t="s">
-        <v>85</v>
+        <v>72</v>
       </c>
       <c r="K7" s="0" t="s">
         <v>36</v>

</xml_diff>

<commit_message>
priyanka kale solved trello defects
</commit_message>
<xml_diff>
--- a/admin/public/products.xlsx
+++ b/admin/public/products.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="124">
   <si>
     <t xml:space="preserve">vendorID</t>
   </si>
@@ -531,8 +531,8 @@
   </sheetPr>
   <dimension ref="A1:AMJ7"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="J3" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="N7" activeCellId="0" sqref="N7"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -552,7 +552,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="0" width="20.94"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="0" width="18.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="0" width="9.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="0" width="10.88"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="0" width="10.87"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="0" width="13.37"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="0" width="15.08"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="22" style="0" width="16.28"/>
@@ -697,13 +697,16 @@
       <c r="R2" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="S2" s="5" t="b">
+      <c r="S2" s="5" t="n">
+        <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="T2" s="5" t="b">
+      <c r="T2" s="5" t="n">
+        <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="U2" s="5" t="b">
+      <c r="U2" s="5" t="n">
+        <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="V2" s="3" t="s">
@@ -732,9 +735,7 @@
       <c r="A3" s="0" t="n">
         <v>101</v>
       </c>
-      <c r="B3" s="3" t="s">
-        <v>28</v>
-      </c>
+      <c r="B3" s="3"/>
       <c r="C3" s="3" t="s">
         <v>29</v>
       </c>
@@ -777,13 +778,16 @@
       <c r="R3" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="S3" s="5" t="b">
+      <c r="S3" s="5" t="n">
+        <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="T3" s="5" t="b">
+      <c r="T3" s="5" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="U3" s="5" t="b">
+      <c r="U3" s="5" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="V3" s="3" t="s">
@@ -854,13 +858,16 @@
       <c r="R4" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="S4" s="5" t="b">
+      <c r="S4" s="5" t="n">
+        <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="T4" s="5" t="b">
+      <c r="T4" s="5" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="U4" s="5" t="b">
+      <c r="U4" s="5" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="V4" s="3" t="s">
@@ -931,13 +938,16 @@
       <c r="R5" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="S5" s="5" t="b">
+      <c r="S5" s="5" t="n">
+        <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="T5" s="5" t="b">
+      <c r="T5" s="5" t="n">
+        <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="U5" s="5" t="b">
+      <c r="U5" s="5" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="V5" s="3" t="s">
@@ -1008,13 +1018,16 @@
       <c r="R6" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="S6" s="5" t="b">
+      <c r="S6" s="5" t="n">
+        <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="T6" s="5" t="b">
+      <c r="T6" s="5" t="n">
+        <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="U6" s="5" t="b">
+      <c r="U6" s="5" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="V6" s="3" t="s">
@@ -1083,13 +1096,16 @@
       <c r="R7" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="S7" s="5" t="b">
+      <c r="S7" s="5" t="n">
+        <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="T7" s="5" t="b">
+      <c r="T7" s="5" t="n">
+        <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="U7" s="5" t="b">
+      <c r="U7" s="5" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="V7" s="3" t="s">

</xml_diff>

<commit_message>
Priyanka k solved defects
</commit_message>
<xml_diff>
--- a/admin/public/products.xlsx
+++ b/admin/public/products.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="123">
   <si>
     <t xml:space="preserve">vendorID</t>
   </si>
@@ -68,12 +68,6 @@
     <t xml:space="preserve">availableQuantity</t>
   </si>
   <si>
-    <t xml:space="preserve">productYTubeVideo</t>
-  </si>
-  <si>
-    <t xml:space="preserve">productVideoType</t>
-  </si>
-  <si>
     <t xml:space="preserve">status</t>
   </si>
   <si>
@@ -86,16 +80,19 @@
     <t xml:space="preserve">newProduct</t>
   </si>
   <si>
+    <t xml:space="preserve">bestSeller</t>
+  </si>
+  <si>
     <t xml:space="preserve">unit</t>
   </si>
   <si>
-    <t xml:space="preserve">featureList1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">featureList2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">featureList3</t>
+    <t xml:space="preserve">feature1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">feature2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">feature3</t>
   </si>
   <si>
     <t xml:space="preserve">size</t>
@@ -531,8 +528,8 @@
   </sheetPr>
   <dimension ref="A1:AMJ7"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="P1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="X2" activeCellId="0" sqref="X2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -549,16 +546,15 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="13.28"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="13" style="0" width="15.99"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="18.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="0" width="20.94"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="0" width="18.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="0" width="9.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="0" width="10.87"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="0" width="13.37"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="0" width="15.08"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="22" style="0" width="16.28"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="24" min="23" style="0" width="23.72"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="25" min="25" style="0" width="20.22"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="26" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="0" width="9.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="0" width="10.87"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="0" width="13.37"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="0" width="15.08"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="20" style="0" width="16.28"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="23" min="22" style="0" width="23.72"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="24" min="24" style="0" width="20.22"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1023" min="25" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1024" style="0" width="9.14"/>
   </cols>
   <sheetData>
     <row r="1" s="1" customFormat="true" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -634,7 +630,7 @@
       <c r="X1" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="Y1" s="2" t="s">
+      <c r="Y1" s="1" t="s">
         <v>24</v>
       </c>
       <c r="Z1" s="1" t="s">
@@ -643,9 +639,7 @@
       <c r="AA1" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="AB1" s="1" t="s">
-        <v>27</v>
-      </c>
+      <c r="AMI1" s="0"/>
       <c r="AMJ1" s="0"/>
     </row>
     <row r="2" customFormat="false" ht="123.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -653,32 +647,32 @@
         <v>101</v>
       </c>
       <c r="B2" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2" s="3" t="s">
         <v>28</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>29</v>
       </c>
       <c r="D2" s="3"/>
       <c r="E2" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="F2" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="F2" s="3" t="s">
+      <c r="G2" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="G2" s="3" t="s">
+      <c r="H2" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="H2" s="3" t="s">
+      <c r="I2" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="I2" s="3" t="s">
+      <c r="J2" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="J2" s="3" t="s">
+      <c r="K2" s="3" t="s">
         <v>35</v>
-      </c>
-      <c r="K2" s="3" t="s">
-        <v>36</v>
       </c>
       <c r="L2" s="4" t="n">
         <v>9999</v>
@@ -692,10 +686,16 @@
       <c r="O2" s="3" t="n">
         <v>4</v>
       </c>
-      <c r="P2" s="3"/>
-      <c r="Q2" s="3"/>
-      <c r="R2" s="3" t="s">
-        <v>37</v>
+      <c r="P2" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="Q2" s="5" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="R2" s="5" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
       </c>
       <c r="S2" s="5" t="n">
         <f aca="false">TRUE()</f>
@@ -705,9 +705,8 @@
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="U2" s="5" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
+      <c r="U2" s="3" t="s">
+        <v>37</v>
       </c>
       <c r="V2" s="3" t="s">
         <v>38</v>
@@ -718,48 +717,47 @@
       <c r="X2" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="Y2" s="3" t="s">
+      <c r="Y2" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="Z2" s="6" t="s">
+      <c r="Z2" s="0" t="s">
         <v>42</v>
       </c>
-      <c r="AA2" s="0" t="s">
+      <c r="AA2" s="3" t="s">
         <v>43</v>
-      </c>
-      <c r="AB2" s="3" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="105.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="n">
         <v>101</v>
       </c>
-      <c r="B3" s="3"/>
+      <c r="B3" s="3" t="s">
+        <v>27</v>
+      </c>
       <c r="C3" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D3" s="3"/>
       <c r="E3" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F3" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="G3" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="G3" s="3" t="s">
+      <c r="H3" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="H3" s="3" t="s">
+      <c r="I3" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="I3" s="3" t="s">
+      <c r="J3" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="J3" s="3" t="s">
-        <v>49</v>
-      </c>
       <c r="K3" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="L3" s="3" t="n">
         <v>8999</v>
@@ -773,25 +771,30 @@
       <c r="O3" s="3" t="n">
         <v>4</v>
       </c>
-      <c r="P3" s="3"/>
-      <c r="Q3" s="3"/>
-      <c r="R3" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="S3" s="5" t="n">
+      <c r="P3" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="Q3" s="5" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
+      </c>
+      <c r="R3" s="5" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="S3" s="5" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
       </c>
       <c r="T3" s="5" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="U3" s="5" t="n">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
+      <c r="U3" s="3" t="s">
+        <v>37</v>
       </c>
       <c r="V3" s="3" t="s">
-        <v>38</v>
+        <v>49</v>
       </c>
       <c r="W3" s="3" t="s">
         <v>50</v>
@@ -799,14 +802,11 @@
       <c r="X3" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="Y3" s="3" t="s">
+      <c r="Y3" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="Z3" s="0" t="s">
         <v>52</v>
-      </c>
-      <c r="Z3" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="AA3" s="0" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="87.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -814,32 +814,32 @@
         <v>101</v>
       </c>
       <c r="B4" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C4" s="3" t="s">
         <v>28</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>29</v>
       </c>
       <c r="D4" s="3"/>
       <c r="E4" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="F4" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="F4" s="3" t="s">
+      <c r="G4" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="G4" s="3" t="s">
+      <c r="H4" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="H4" s="3" t="s">
+      <c r="I4" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="I4" s="3" t="s">
+      <c r="J4" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="J4" s="3" t="s">
-        <v>59</v>
-      </c>
       <c r="K4" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="L4" s="3" t="n">
         <v>12999</v>
@@ -853,25 +853,30 @@
       <c r="O4" s="3" t="n">
         <v>4</v>
       </c>
-      <c r="P4" s="3"/>
-      <c r="Q4" s="3"/>
-      <c r="R4" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="S4" s="5" t="n">
+      <c r="P4" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="Q4" s="5" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
+      </c>
+      <c r="R4" s="5" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="S4" s="5" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
       </c>
       <c r="T4" s="5" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="U4" s="5" t="n">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
+      <c r="U4" s="3" t="s">
+        <v>37</v>
       </c>
       <c r="V4" s="3" t="s">
-        <v>38</v>
+        <v>59</v>
       </c>
       <c r="W4" s="3" t="s">
         <v>60</v>
@@ -879,14 +884,11 @@
       <c r="X4" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="Y4" s="3" t="s">
+      <c r="Y4" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="Z4" s="0" t="s">
         <v>62</v>
-      </c>
-      <c r="Z4" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="AA4" s="0" t="s">
-        <v>63</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="69.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -894,34 +896,34 @@
         <v>101</v>
       </c>
       <c r="B5" s="0" t="s">
+        <v>63</v>
+      </c>
+      <c r="C5" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="D5" s="0" t="s">
         <v>65</v>
       </c>
-      <c r="D5" s="0" t="s">
+      <c r="E5" s="0" t="s">
         <v>66</v>
       </c>
-      <c r="E5" s="0" t="s">
+      <c r="F5" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="F5" s="3" t="s">
+      <c r="G5" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="G5" s="3" t="s">
+      <c r="H5" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="H5" s="3" t="s">
+      <c r="I5" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="I5" s="3" t="s">
+      <c r="J5" s="0" t="s">
         <v>71</v>
       </c>
-      <c r="J5" s="0" t="s">
-        <v>72</v>
-      </c>
       <c r="K5" s="0" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="L5" s="0" t="n">
         <v>899</v>
@@ -935,25 +937,32 @@
       <c r="O5" s="0" t="n">
         <v>3</v>
       </c>
-      <c r="R5" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="S5" s="5" t="n">
+      <c r="P5" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="Q5" s="5" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="T5" s="5" t="n">
+      <c r="R5" s="5" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="U5" s="5" t="n">
+      <c r="S5" s="5" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
+      <c r="T5" s="5" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="U5" s="3" t="s">
+        <v>37</v>
+      </c>
       <c r="V5" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="W5" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="W5" s="0" t="s">
         <v>73</v>
       </c>
       <c r="X5" s="0" t="s">
@@ -963,45 +972,42 @@
         <v>75</v>
       </c>
       <c r="Z5" s="0" t="s">
-        <v>76</v>
-      </c>
-      <c r="AA5" s="0" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="69.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="n">
         <v>101</v>
       </c>
       <c r="B6" s="0" t="s">
+        <v>63</v>
+      </c>
+      <c r="C6" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="C6" s="3" t="s">
+      <c r="D6" s="0" t="s">
         <v>65</v>
       </c>
-      <c r="D6" s="0" t="s">
+      <c r="E6" s="0" t="s">
         <v>66</v>
       </c>
-      <c r="E6" s="0" t="s">
+      <c r="F6" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="F6" s="3" t="s">
-        <v>68</v>
-      </c>
       <c r="G6" s="3" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="H6" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="I6" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="I6" s="3" t="s">
+      <c r="J6" s="0" t="s">
         <v>71</v>
       </c>
-      <c r="J6" s="0" t="s">
-        <v>72</v>
-      </c>
       <c r="K6" s="0" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="L6" s="0" t="n">
         <v>899</v>
@@ -1015,38 +1021,39 @@
       <c r="O6" s="0" t="n">
         <v>3</v>
       </c>
-      <c r="R6" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="S6" s="5" t="n">
+      <c r="P6" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="Q6" s="5" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="T6" s="5" t="n">
+      <c r="R6" s="5" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="U6" s="5" t="n">
+      <c r="S6" s="5" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
+      <c r="T6" s="5"/>
+      <c r="U6" s="3" t="s">
+        <v>37</v>
+      </c>
       <c r="V6" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="W6" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="W6" s="0" t="s">
         <v>73</v>
       </c>
       <c r="X6" s="0" t="s">
         <v>74</v>
       </c>
       <c r="Y6" s="0" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="Z6" s="0" t="s">
-        <v>78</v>
-      </c>
-      <c r="AA6" s="0" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1054,34 +1061,34 @@
         <v>101</v>
       </c>
       <c r="B7" s="0" t="s">
+        <v>78</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="D7" s="6" t="s">
         <v>79</v>
       </c>
-      <c r="C7" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="D7" s="6" t="s">
+      <c r="E7" s="0" t="s">
         <v>80</v>
       </c>
-      <c r="E7" s="0" t="s">
+      <c r="F7" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="F7" s="3" t="s">
+      <c r="G7" s="3" t="s">
         <v>82</v>
       </c>
-      <c r="G7" s="3" t="s">
+      <c r="H7" s="6" t="s">
         <v>83</v>
       </c>
-      <c r="H7" s="6" t="s">
+      <c r="I7" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="I7" s="3" t="s">
-        <v>85</v>
-      </c>
       <c r="J7" s="3" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="K7" s="0" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="L7" s="0" t="n">
         <v>1199</v>
@@ -1093,43 +1100,44 @@
       <c r="O7" s="0" t="n">
         <v>4</v>
       </c>
-      <c r="R7" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="S7" s="5" t="n">
+      <c r="P7" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="Q7" s="5" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="T7" s="5" t="n">
+      <c r="R7" s="5" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="U7" s="5" t="n">
+      <c r="S7" s="5" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
+      <c r="T7" s="5"/>
+      <c r="U7" s="3" t="s">
+        <v>37</v>
+      </c>
       <c r="V7" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="W7" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="W7" s="0" t="s">
         <v>73</v>
       </c>
       <c r="X7" s="0" t="s">
         <v>74</v>
       </c>
-      <c r="Y7" s="0" t="s">
-        <v>75</v>
-      </c>
-      <c r="Z7" s="6" t="s">
-        <v>78</v>
-      </c>
-      <c r="AA7" s="0" t="s">
-        <v>86</v>
+      <c r="Y7" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="Z7" s="0" t="s">
+        <v>85</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="4">
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="R1:R7" type="list">
+    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="P1:P7" type="list">
       <formula1>"Draft,Publish,Unpublish"</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -1137,11 +1145,11 @@
       <formula1>"inr,usd,eur,gbp"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="S2:U7" type="list">
+    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="Q2:T7" type="list">
       <formula1>"true,false"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="V2:V7" type="list">
+    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="U2:U7" type="list">
       <formula1>"Single,Dozen,Kilograms,Miligrams,Liters,Mililiters"</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -1178,54 +1186,54 @@
   <sheetData>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
+        <v>86</v>
+      </c>
+      <c r="B2" s="0" t="s">
         <v>87</v>
       </c>
-      <c r="B2" s="0" t="s">
+      <c r="C2" s="0" t="s">
         <v>88</v>
       </c>
-      <c r="C2" s="0" t="s">
+      <c r="D2" s="0" t="s">
         <v>89</v>
       </c>
-      <c r="D2" s="0" t="s">
+      <c r="E2" s="0" t="s">
         <v>90</v>
       </c>
-      <c r="E2" s="0" t="s">
+      <c r="F2" s="0" t="s">
         <v>91</v>
       </c>
-      <c r="F2" s="0" t="s">
+      <c r="G2" s="0" t="s">
         <v>92</v>
       </c>
-      <c r="G2" s="0" t="s">
+      <c r="H2" s="0" t="s">
         <v>93</v>
       </c>
-      <c r="H2" s="0" t="s">
+      <c r="I2" s="0" t="s">
         <v>94</v>
       </c>
-      <c r="I2" s="0" t="s">
+      <c r="J2" s="0" t="s">
         <v>95</v>
       </c>
-      <c r="J2" s="0" t="s">
+      <c r="K2" s="0" t="s">
         <v>96</v>
       </c>
-      <c r="K2" s="0" t="s">
+      <c r="L2" s="0" t="s">
         <v>97</v>
       </c>
-      <c r="L2" s="0" t="s">
+      <c r="M2" s="0" t="s">
         <v>98</v>
       </c>
-      <c r="M2" s="0" t="s">
+      <c r="N2" s="0" t="s">
         <v>99</v>
       </c>
-      <c r="N2" s="0" t="s">
+      <c r="O2" s="0" t="s">
         <v>100</v>
-      </c>
-      <c r="O2" s="0" t="s">
-        <v>101</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E3" s="0" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="F3" s="0" t="n">
         <v>15</v>
@@ -1240,125 +1248,125 @@
         <v>75</v>
       </c>
       <c r="J3" s="0" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="K3" s="0" t="n">
         <v>10</v>
       </c>
       <c r="L3" s="0" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F4" s="0" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F5" s="0" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F6" s="0" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F7" s="0" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C8" s="0" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C9" s="0" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C10" s="0" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C11" s="0" t="s">
+        <v>108</v>
+      </c>
+      <c r="D11" s="0" t="s">
         <v>109</v>
-      </c>
-      <c r="D11" s="0" t="s">
-        <v>110</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C12" s="0" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D12" s="0" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C13" s="0" t="s">
+        <v>106</v>
+      </c>
+      <c r="D13" s="0" t="s">
         <v>107</v>
-      </c>
-      <c r="D13" s="0" t="s">
-        <v>108</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C14" s="0" t="s">
+        <v>107</v>
+      </c>
+      <c r="D14" s="0" t="s">
         <v>108</v>
-      </c>
-      <c r="D14" s="0" t="s">
-        <v>109</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C15" s="0" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C16" s="0" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C17" s="0" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C18" s="0" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C19" s="0" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C20" s="0" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C21" s="0" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C22" s="0" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C23" s="0" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1373,65 +1381,65 @@
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H30" s="0" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H31" s="0" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H32" s="0" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H33" s="0" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H34" s="0" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H35" s="0" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H36" s="0" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H37" s="0" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H38" s="0" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H39" s="0" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H40" s="0" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H41" s="0" t="s">
+        <v>121</v>
+      </c>
+      <c r="I41" s="0" t="s">
         <v>122</v>
-      </c>
-      <c r="I41" s="0" t="s">
-        <v>123</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Priyanka kale solved defect
</commit_message>
<xml_diff>
--- a/admin/public/products.xlsx
+++ b/admin/public/products.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="121">
   <si>
     <t xml:space="preserve">vendorID</t>
   </si>
@@ -68,9 +68,6 @@
     <t xml:space="preserve">availableQuantity</t>
   </si>
   <si>
-    <t xml:space="preserve">status</t>
-  </si>
-  <si>
     <t xml:space="preserve">featured</t>
   </si>
   <si>
@@ -129,9 +126,6 @@
   </si>
   <si>
     <t xml:space="preserve">inr</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Publish</t>
   </si>
   <si>
     <t xml:space="preserve">Single</t>
@@ -528,8 +522,8 @@
   </sheetPr>
   <dimension ref="A1:AMJ7"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="P1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="X2" activeCellId="0" sqref="X2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="N1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="P1" activeCellId="0" sqref="P1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -546,15 +540,14 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="13.28"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="13" style="0" width="15.99"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="18.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="0" width="9.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="0" width="10.87"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="0" width="13.37"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="0" width="15.08"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="20" style="0" width="16.28"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="23" min="22" style="0" width="23.72"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="24" min="24" style="0" width="20.22"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1023" min="25" style="0" width="8.53"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1024" style="0" width="9.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="0" width="10.87"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="0" width="13.37"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="0" width="15.08"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="19" style="0" width="16.28"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="21" style="0" width="23.72"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="23" min="23" style="0" width="20.22"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1022" min="24" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1023" style="0" width="9.14"/>
   </cols>
   <sheetData>
     <row r="1" s="1" customFormat="true" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -627,7 +620,7 @@
       <c r="W1" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="X1" s="2" t="s">
+      <c r="X1" s="1" t="s">
         <v>23</v>
       </c>
       <c r="Y1" s="1" t="s">
@@ -636,43 +629,41 @@
       <c r="Z1" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="AA1" s="1" t="s">
-        <v>26</v>
-      </c>
+      <c r="AMH1" s="0"/>
       <c r="AMI1" s="0"/>
       <c r="AMJ1" s="0"/>
     </row>
-    <row r="2" customFormat="false" ht="123.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="122.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="n">
         <v>101</v>
       </c>
       <c r="B2" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C2" s="3" t="s">
         <v>27</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>28</v>
       </c>
       <c r="D2" s="3"/>
       <c r="E2" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="F2" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="F2" s="3" t="s">
+      <c r="G2" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="G2" s="3" t="s">
+      <c r="H2" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="H2" s="3" t="s">
+      <c r="I2" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="I2" s="3" t="s">
+      <c r="J2" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="J2" s="3" t="s">
+      <c r="K2" s="3" t="s">
         <v>34</v>
-      </c>
-      <c r="K2" s="3" t="s">
-        <v>35</v>
       </c>
       <c r="L2" s="4" t="n">
         <v>9999</v>
@@ -686,8 +677,9 @@
       <c r="O2" s="3" t="n">
         <v>4</v>
       </c>
-      <c r="P2" s="3" t="s">
-        <v>36</v>
+      <c r="P2" s="5" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
       </c>
       <c r="Q2" s="5" t="n">
         <f aca="false">TRUE()</f>
@@ -701,30 +693,26 @@
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="T2" s="5" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
+      <c r="T2" s="3" t="s">
+        <v>35</v>
       </c>
       <c r="U2" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="V2" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="V2" s="3" t="s">
+      <c r="W2" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="W2" s="3" t="s">
+      <c r="X2" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="X2" s="3" t="s">
+      <c r="Y2" s="0" t="s">
         <v>40</v>
       </c>
-      <c r="Y2" s="6" t="s">
+      <c r="Z2" s="3" t="s">
         <v>41</v>
-      </c>
-      <c r="Z2" s="0" t="s">
-        <v>42</v>
-      </c>
-      <c r="AA2" s="3" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="105.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -732,32 +720,32 @@
         <v>101</v>
       </c>
       <c r="B3" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C3" s="3" t="s">
         <v>27</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>28</v>
       </c>
       <c r="D3" s="3"/>
       <c r="E3" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F3" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="H3" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="G3" s="3" t="s">
+      <c r="I3" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="H3" s="3" t="s">
+      <c r="J3" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="I3" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="J3" s="3" t="s">
-        <v>48</v>
-      </c>
       <c r="K3" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="L3" s="3" t="n">
         <v>8999</v>
@@ -771,12 +759,13 @@
       <c r="O3" s="3" t="n">
         <v>4</v>
       </c>
-      <c r="P3" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="Q3" s="5" t="n">
+      <c r="P3" s="5" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
+      </c>
+      <c r="Q3" s="5" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
       </c>
       <c r="R3" s="5" t="n">
         <f aca="false">FALSE()</f>
@@ -786,27 +775,23 @@
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="T3" s="5" t="n">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
+      <c r="T3" s="3" t="s">
+        <v>35</v>
       </c>
       <c r="U3" s="3" t="s">
-        <v>37</v>
+        <v>47</v>
       </c>
       <c r="V3" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="W3" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="W3" s="3" t="s">
+      <c r="X3" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="Y3" s="0" t="s">
         <v>50</v>
-      </c>
-      <c r="X3" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="Y3" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="Z3" s="0" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="87.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -814,32 +799,32 @@
         <v>101</v>
       </c>
       <c r="B4" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C4" s="3" t="s">
         <v>27</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>28</v>
       </c>
       <c r="D4" s="3"/>
       <c r="E4" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="G4" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="F4" s="3" t="s">
+      <c r="H4" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="G4" s="3" t="s">
+      <c r="I4" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="H4" s="3" t="s">
+      <c r="J4" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="I4" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="J4" s="3" t="s">
-        <v>58</v>
-      </c>
       <c r="K4" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="L4" s="3" t="n">
         <v>12999</v>
@@ -853,12 +838,13 @@
       <c r="O4" s="3" t="n">
         <v>4</v>
       </c>
-      <c r="P4" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="Q4" s="5" t="n">
+      <c r="P4" s="5" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
+      </c>
+      <c r="Q4" s="5" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
       </c>
       <c r="R4" s="5" t="n">
         <f aca="false">FALSE()</f>
@@ -868,62 +854,58 @@
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="T4" s="5" t="n">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
+      <c r="T4" s="3" t="s">
+        <v>35</v>
       </c>
       <c r="U4" s="3" t="s">
-        <v>37</v>
+        <v>57</v>
       </c>
       <c r="V4" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="W4" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="W4" s="3" t="s">
+      <c r="X4" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="Y4" s="0" t="s">
         <v>60</v>
       </c>
-      <c r="X4" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="Y4" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="Z4" s="0" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="69.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="5" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="n">
         <v>101</v>
       </c>
       <c r="B5" s="0" t="s">
+        <v>61</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="D5" s="0" t="s">
         <v>63</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="E5" s="0" t="s">
         <v>64</v>
       </c>
-      <c r="D5" s="0" t="s">
+      <c r="F5" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="E5" s="0" t="s">
+      <c r="G5" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="F5" s="3" t="s">
+      <c r="H5" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="G5" s="3" t="s">
+      <c r="I5" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="H5" s="3" t="s">
+      <c r="J5" s="0" t="s">
         <v>69</v>
       </c>
-      <c r="I5" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="J5" s="0" t="s">
-        <v>71</v>
-      </c>
       <c r="K5" s="0" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="L5" s="0" t="n">
         <v>899</v>
@@ -937,42 +919,39 @@
       <c r="O5" s="0" t="n">
         <v>3</v>
       </c>
-      <c r="P5" s="3" t="s">
-        <v>36</v>
+      <c r="P5" s="5" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
       </c>
       <c r="Q5" s="5" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="R5" s="5" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
+        <f aca="false">FALSE()</f>
+        <v>0</v>
       </c>
       <c r="S5" s="5" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="T5" s="5" t="n">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
+      <c r="T5" s="3" t="s">
+        <v>35</v>
       </c>
       <c r="U5" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="V5" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="V5" s="0" t="s">
+        <v>71</v>
+      </c>
+      <c r="W5" s="0" t="s">
         <v>72</v>
       </c>
-      <c r="W5" s="0" t="s">
+      <c r="X5" s="0" t="s">
         <v>73</v>
       </c>
-      <c r="X5" s="0" t="s">
-        <v>74</v>
-      </c>
       <c r="Y5" s="0" t="s">
-        <v>75</v>
-      </c>
-      <c r="Z5" s="0" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -980,34 +959,34 @@
         <v>101</v>
       </c>
       <c r="B6" s="0" t="s">
+        <v>61</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="D6" s="0" t="s">
         <v>63</v>
       </c>
-      <c r="C6" s="3" t="s">
+      <c r="E6" s="0" t="s">
         <v>64</v>
       </c>
-      <c r="D6" s="0" t="s">
+      <c r="F6" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="E6" s="0" t="s">
-        <v>66</v>
-      </c>
-      <c r="F6" s="3" t="s">
+      <c r="G6" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="H6" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="G6" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="H6" s="3" t="s">
+      <c r="I6" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="J6" s="0" t="s">
         <v>69</v>
       </c>
-      <c r="I6" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="J6" s="0" t="s">
-        <v>71</v>
-      </c>
       <c r="K6" s="0" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="L6" s="0" t="n">
         <v>899</v>
@@ -1021,39 +1000,36 @@
       <c r="O6" s="0" t="n">
         <v>3</v>
       </c>
-      <c r="P6" s="3" t="s">
-        <v>36</v>
+      <c r="P6" s="5" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
       </c>
       <c r="Q6" s="5" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="R6" s="5" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="S6" s="5" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="T6" s="5"/>
+      <c r="S6" s="5"/>
+      <c r="T6" s="3" t="s">
+        <v>35</v>
+      </c>
       <c r="U6" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="V6" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="V6" s="0" t="s">
+        <v>71</v>
+      </c>
+      <c r="W6" s="0" t="s">
         <v>72</v>
       </c>
-      <c r="W6" s="0" t="s">
-        <v>73</v>
-      </c>
       <c r="X6" s="0" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="Y6" s="0" t="s">
-        <v>77</v>
-      </c>
-      <c r="Z6" s="0" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1061,34 +1037,34 @@
         <v>101</v>
       </c>
       <c r="B7" s="0" t="s">
+        <v>76</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="D7" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="E7" s="0" t="s">
         <v>78</v>
       </c>
-      <c r="C7" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="D7" s="6" t="s">
+      <c r="F7" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="E7" s="0" t="s">
+      <c r="G7" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="F7" s="3" t="s">
+      <c r="H7" s="6" t="s">
         <v>81</v>
       </c>
-      <c r="G7" s="3" t="s">
+      <c r="I7" s="3" t="s">
         <v>82</v>
       </c>
-      <c r="H7" s="6" t="s">
-        <v>83</v>
-      </c>
-      <c r="I7" s="3" t="s">
-        <v>84</v>
-      </c>
       <c r="J7" s="3" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="K7" s="0" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="L7" s="0" t="n">
         <v>1199</v>
@@ -1100,56 +1076,49 @@
       <c r="O7" s="0" t="n">
         <v>4</v>
       </c>
-      <c r="P7" s="3" t="s">
-        <v>36</v>
+      <c r="P7" s="5" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
       </c>
       <c r="Q7" s="5" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="R7" s="5" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="S7" s="5" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="T7" s="5"/>
+      <c r="S7" s="5"/>
+      <c r="T7" s="3" t="s">
+        <v>35</v>
+      </c>
       <c r="U7" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="V7" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="V7" s="0" t="s">
+        <v>71</v>
+      </c>
+      <c r="W7" s="0" t="s">
         <v>72</v>
       </c>
-      <c r="W7" s="0" t="s">
-        <v>73</v>
-      </c>
-      <c r="X7" s="0" t="s">
-        <v>74</v>
-      </c>
-      <c r="Y7" s="6" t="s">
-        <v>77</v>
-      </c>
-      <c r="Z7" s="0" t="s">
-        <v>85</v>
+      <c r="X7" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="Y7" s="0" t="s">
+        <v>83</v>
       </c>
     </row>
   </sheetData>
-  <dataValidations count="4">
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="P1:P7" type="list">
-      <formula1>"Draft,Publish,Unpublish"</formula1>
-      <formula2>0</formula2>
-    </dataValidation>
+  <dataValidations count="3">
     <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="K2:K4" type="list">
       <formula1>"inr,usd,eur,gbp"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="Q2:T7" type="list">
+    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="P2:S7" type="list">
       <formula1>"true,false"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="U2:U7" type="list">
+    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="T2:T7" type="list">
       <formula1>"Single,Dozen,Kilograms,Miligrams,Liters,Mililiters"</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -1186,54 +1155,54 @@
   <sheetData>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
+        <v>84</v>
+      </c>
+      <c r="B2" s="0" t="s">
+        <v>85</v>
+      </c>
+      <c r="C2" s="0" t="s">
         <v>86</v>
       </c>
-      <c r="B2" s="0" t="s">
+      <c r="D2" s="0" t="s">
         <v>87</v>
       </c>
-      <c r="C2" s="0" t="s">
+      <c r="E2" s="0" t="s">
         <v>88</v>
       </c>
-      <c r="D2" s="0" t="s">
+      <c r="F2" s="0" t="s">
         <v>89</v>
       </c>
-      <c r="E2" s="0" t="s">
+      <c r="G2" s="0" t="s">
         <v>90</v>
       </c>
-      <c r="F2" s="0" t="s">
+      <c r="H2" s="0" t="s">
         <v>91</v>
       </c>
-      <c r="G2" s="0" t="s">
+      <c r="I2" s="0" t="s">
         <v>92</v>
       </c>
-      <c r="H2" s="0" t="s">
+      <c r="J2" s="0" t="s">
         <v>93</v>
       </c>
-      <c r="I2" s="0" t="s">
+      <c r="K2" s="0" t="s">
         <v>94</v>
       </c>
-      <c r="J2" s="0" t="s">
+      <c r="L2" s="0" t="s">
         <v>95</v>
       </c>
-      <c r="K2" s="0" t="s">
+      <c r="M2" s="0" t="s">
         <v>96</v>
       </c>
-      <c r="L2" s="0" t="s">
+      <c r="N2" s="0" t="s">
         <v>97</v>
       </c>
-      <c r="M2" s="0" t="s">
+      <c r="O2" s="0" t="s">
         <v>98</v>
-      </c>
-      <c r="N2" s="0" t="s">
-        <v>99</v>
-      </c>
-      <c r="O2" s="0" t="s">
-        <v>100</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E3" s="0" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="F3" s="0" t="n">
         <v>15</v>
@@ -1248,125 +1217,125 @@
         <v>75</v>
       </c>
       <c r="J3" s="0" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="K3" s="0" t="n">
         <v>10</v>
       </c>
       <c r="L3" s="0" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F4" s="0" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F5" s="0" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F6" s="0" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F7" s="0" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C8" s="0" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C9" s="0" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C10" s="0" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C11" s="0" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="D11" s="0" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C12" s="0" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="D12" s="0" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C13" s="0" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="D13" s="0" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C14" s="0" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="D14" s="0" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C15" s="0" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C16" s="0" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C17" s="0" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C18" s="0" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C19" s="0" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C20" s="0" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C21" s="0" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C22" s="0" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C23" s="0" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1381,65 +1350,65 @@
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H30" s="0" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H31" s="0" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H32" s="0" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H33" s="0" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H34" s="0" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H35" s="0" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H36" s="0" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H37" s="0" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H38" s="0" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H39" s="0" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H40" s="0" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H41" s="0" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="I41" s="0" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
priyanka kale solved critical defect
</commit_message>
<xml_diff>
--- a/admin/public/products.xlsx
+++ b/admin/public/products.xlsx
@@ -21,10 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="122">
-  <si>
-    <t xml:space="preserve">vendorID</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="122">
   <si>
     <t xml:space="preserve">section</t>
   </si>
@@ -276,6 +273,9 @@
   </si>
   <si>
     <t xml:space="preserve">#ec47cd</t>
+  </si>
+  <si>
+    <t xml:space="preserve">     AB005-1</t>
   </si>
   <si>
     <t xml:space="preserve">PID</t>
@@ -478,12 +478,12 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
@@ -508,12 +508,12 @@
     </xf>
   </cellXfs>
   <cellStyles count="6">
-    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Comma" xfId="15" builtinId="3"/>
+    <cellStyle name="Comma [0]" xfId="16" builtinId="6"/>
+    <cellStyle name="Currency" xfId="17" builtinId="4"/>
+    <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
+    <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
 </styleSheet>
 </file>
@@ -523,130 +523,128 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AMJ7"/>
+  <dimension ref="A1:AMJ8"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A3" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C7" activeCellId="0" sqref="C7"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B5" activeCellId="0" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="20"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="16.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="19.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="14.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="7" style="0" width="23"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="56.72"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="21.28"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="10.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="13.28"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="13" style="0" width="15.99"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="18.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="0" width="10.87"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="0" width="13.37"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="0" width="15.08"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="19" style="0" width="16.28"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="21" style="0" width="23.72"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="23" min="23" style="0" width="20.22"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1022" min="24" style="0" width="8.53"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1023" style="0" width="9.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="20"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="16.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="19.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="14.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="6" style="0" width="23"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="56.72"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="21.28"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="10.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="13.28"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="12" style="0" width="15.99"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="18.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="10.87"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="0" width="13.37"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="0" width="15.08"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="18" style="0" width="16.28"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="20" style="0" width="23.72"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="22" style="0" width="20.22"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1021" min="23" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1022" style="0" width="9.14"/>
   </cols>
   <sheetData>
-    <row r="1" s="1" customFormat="true" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" s="2" customFormat="true" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="2" t="s">
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="H1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="I1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="J1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="K1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="2" t="s">
+      <c r="L1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="2" t="s">
+      <c r="M1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="2" t="s">
+      <c r="N1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="2" t="s">
+      <c r="O1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="2" t="s">
+      <c r="P1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="2" t="s">
+      <c r="Q1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="R1" s="2" t="s">
+      <c r="R1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="S1" s="2" t="s">
+      <c r="S1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="T1" s="2" t="s">
+      <c r="T1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="U1" s="2" t="s">
+      <c r="U1" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="V1" s="2" t="s">
+      <c r="V1" s="1" t="s">
         <v>21</v>
       </c>
       <c r="W1" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="X1" s="1" t="s">
+      <c r="X1" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="Y1" s="1" t="s">
+      <c r="Y1" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="Z1" s="1" t="s">
-        <v>25</v>
-      </c>
+      <c r="AMG1" s="0"/>
       <c r="AMH1" s="0"/>
       <c r="AMI1" s="0"/>
       <c r="AMJ1" s="0"/>
     </row>
     <row r="2" customFormat="false" ht="122.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="n">
-        <v>101</v>
+      <c r="A2" s="3" t="s">
+        <v>25</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="3"/>
+      <c r="D2" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="D2" s="3"/>
       <c r="E2" s="3" t="s">
         <v>28</v>
       </c>
@@ -665,20 +663,21 @@
       <c r="J2" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="K2" s="3" t="s">
-        <v>34</v>
+      <c r="K2" s="4" t="n">
+        <v>9999</v>
       </c>
       <c r="L2" s="4" t="n">
-        <v>9999</v>
-      </c>
-      <c r="M2" s="4" t="n">
         <v>20</v>
       </c>
+      <c r="M2" s="3" t="n">
+        <v>8000</v>
+      </c>
       <c r="N2" s="3" t="n">
-        <v>8000</v>
-      </c>
-      <c r="O2" s="3" t="n">
         <v>4</v>
+      </c>
+      <c r="O2" s="5" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
       </c>
       <c r="P2" s="5" t="n">
         <f aca="false">TRUE()</f>
@@ -692,9 +691,8 @@
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="S2" s="5" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
+      <c r="S2" s="3" t="s">
+        <v>34</v>
       </c>
       <c r="T2" s="3" t="s">
         <v>35</v>
@@ -705,32 +703,29 @@
       <c r="V2" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="W2" s="3" t="s">
+      <c r="W2" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="X2" s="6" t="s">
+      <c r="X2" s="0" t="s">
         <v>39</v>
       </c>
-      <c r="Y2" s="0" t="s">
+      <c r="Y2" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="Z2" s="3" t="s">
-        <v>41</v>
-      </c>
     </row>
     <row r="3" customFormat="false" ht="105.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="n">
-        <v>101</v>
+      <c r="A3" s="3" t="s">
+        <v>25</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="C3" s="3"/>
+      <c r="D3" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="D3" s="3"/>
       <c r="E3" s="3" t="s">
-        <v>28</v>
+        <v>41</v>
       </c>
       <c r="F3" s="3" t="s">
         <v>42</v>
@@ -745,26 +740,27 @@
         <v>45</v>
       </c>
       <c r="J3" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="K3" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
+      </c>
+      <c r="K3" s="3" t="n">
+        <v>8999</v>
       </c>
       <c r="L3" s="3" t="n">
-        <v>8999</v>
+        <v>10</v>
       </c>
       <c r="M3" s="3" t="n">
-        <v>10</v>
+        <v>8910</v>
       </c>
       <c r="N3" s="3" t="n">
-        <v>8910</v>
-      </c>
-      <c r="O3" s="3" t="n">
         <v>4</v>
       </c>
+      <c r="O3" s="5" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
       <c r="P3" s="5" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
+        <f aca="false">FALSE()</f>
+        <v>0</v>
       </c>
       <c r="Q3" s="5" t="n">
         <f aca="false">FALSE()</f>
@@ -774,76 +770,73 @@
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="S3" s="5" t="n">
+      <c r="S3" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="T3" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="U3" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="V3" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="W3" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="X3" s="0" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="87.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A4" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C4" s="3"/>
+      <c r="D4" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="H4" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="I4" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="J4" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="K4" s="3" t="n">
+        <v>12999</v>
+      </c>
+      <c r="L4" s="3" t="n">
+        <v>10</v>
+      </c>
+      <c r="M4" s="3" t="n">
+        <v>12997</v>
+      </c>
+      <c r="N4" s="3" t="n">
+        <v>4</v>
+      </c>
+      <c r="O4" s="5" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="P4" s="5" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
-      </c>
-      <c r="T3" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="U3" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="V3" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="W3" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="X3" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="Y3" s="0" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="87.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="n">
-        <v>101</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="D4" s="3"/>
-      <c r="E4" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="F4" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="G4" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="H4" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="I4" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="J4" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="K4" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="L4" s="3" t="n">
-        <v>12999</v>
-      </c>
-      <c r="M4" s="3" t="n">
-        <v>10</v>
-      </c>
-      <c r="N4" s="3" t="n">
-        <v>12997</v>
-      </c>
-      <c r="O4" s="3" t="n">
-        <v>4</v>
-      </c>
-      <c r="P4" s="5" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
       </c>
       <c r="Q4" s="5" t="n">
         <f aca="false">FALSE()</f>
@@ -853,275 +846,335 @@
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="S4" s="5" t="n">
+      <c r="S4" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="T4" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="U4" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="V4" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="W4" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="X4" s="0" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
+        <v>60</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="C5" s="0" t="s">
+        <v>62</v>
+      </c>
+      <c r="D5" s="0" t="s">
+        <v>63</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="H5" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="I5" s="0" t="s">
+        <v>68</v>
+      </c>
+      <c r="J5" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="K5" s="0" t="n">
+        <v>899</v>
+      </c>
+      <c r="L5" s="3" t="n">
+        <v>5</v>
+      </c>
+      <c r="M5" s="3" t="n">
+        <v>855</v>
+      </c>
+      <c r="N5" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="O5" s="5" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="P5" s="5" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="Q5" s="5" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
-      </c>
-      <c r="T4" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="U4" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="V4" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="W4" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="X4" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="Y4" s="0" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="n">
-        <v>101</v>
-      </c>
-      <c r="B5" s="0" t="s">
-        <v>61</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="D5" s="0" t="s">
-        <v>63</v>
-      </c>
-      <c r="E5" s="0" t="s">
-        <v>64</v>
-      </c>
-      <c r="F5" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="G5" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="H5" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="I5" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="J5" s="0" t="s">
-        <v>69</v>
-      </c>
-      <c r="K5" s="0" t="s">
-        <v>34</v>
-      </c>
-      <c r="L5" s="0" t="n">
-        <v>899</v>
-      </c>
-      <c r="M5" s="3" t="n">
-        <v>5</v>
-      </c>
-      <c r="N5" s="3" t="n">
-        <v>855</v>
-      </c>
-      <c r="O5" s="0" t="n">
-        <v>3</v>
-      </c>
-      <c r="P5" s="5" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="Q5" s="5" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
       </c>
       <c r="R5" s="5" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="S5" s="5" t="n">
+      <c r="S5" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="T5" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="U5" s="0" t="s">
+        <v>70</v>
+      </c>
+      <c r="V5" s="0" t="s">
+        <v>71</v>
+      </c>
+      <c r="W5" s="0" t="s">
+        <v>72</v>
+      </c>
+      <c r="X5" s="0" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="s">
+        <v>60</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="C6" s="0" t="s">
+        <v>62</v>
+      </c>
+      <c r="D6" s="0" t="s">
+        <v>63</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="G6" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="H6" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="I6" s="0" t="s">
+        <v>68</v>
+      </c>
+      <c r="J6" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="K6" s="0" t="n">
+        <v>899</v>
+      </c>
+      <c r="L6" s="3" t="n">
+        <v>5</v>
+      </c>
+      <c r="M6" s="3" t="n">
+        <v>855</v>
+      </c>
+      <c r="N6" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="O6" s="5" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="P6" s="5" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="Q6" s="5" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="T5" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="U5" s="3" t="s">
+      <c r="R6" s="5"/>
+      <c r="S6" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="T6" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="U6" s="0" t="s">
         <v>70</v>
       </c>
-      <c r="V5" s="0" t="s">
+      <c r="V6" s="0" t="s">
         <v>71</v>
       </c>
-      <c r="W5" s="0" t="s">
-        <v>72</v>
-      </c>
-      <c r="X5" s="0" t="s">
-        <v>73</v>
-      </c>
-      <c r="Y5" s="0" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="n">
-        <v>101</v>
-      </c>
-      <c r="B6" s="0" t="s">
+      <c r="W6" s="0" t="s">
+        <v>75</v>
+      </c>
+      <c r="X6" s="0" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="s">
+        <v>76</v>
+      </c>
+      <c r="B7" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="C6" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="D6" s="0" t="s">
-        <v>63</v>
-      </c>
-      <c r="E6" s="0" t="s">
-        <v>64</v>
-      </c>
-      <c r="F6" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="G6" s="3" t="s">
-        <v>75</v>
-      </c>
-      <c r="H6" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="I6" s="3" t="s">
+      <c r="C7" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="D7" s="0" t="s">
+        <v>78</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="G7" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="H7" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="I7" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="J6" s="0" t="s">
-        <v>69</v>
-      </c>
-      <c r="K6" s="0" t="s">
-        <v>34</v>
-      </c>
-      <c r="L6" s="0" t="n">
-        <v>899</v>
-      </c>
-      <c r="M6" s="3" t="n">
+      <c r="J7" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="K7" s="0" t="n">
+        <v>1199</v>
+      </c>
+      <c r="L7" s="3" t="n">
         <v>5</v>
       </c>
-      <c r="N6" s="3" t="n">
-        <v>855</v>
-      </c>
-      <c r="O6" s="0" t="n">
-        <v>3</v>
-      </c>
-      <c r="P6" s="5" t="n">
+      <c r="M7" s="3"/>
+      <c r="N7" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="O7" s="5" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="Q6" s="5" t="n">
+      <c r="P7" s="5" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="R6" s="5" t="n">
+      <c r="Q7" s="5" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="S6" s="5"/>
-      <c r="T6" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="U6" s="3" t="s">
+      <c r="R7" s="5"/>
+      <c r="S7" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="T7" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="U7" s="0" t="s">
         <v>70</v>
       </c>
-      <c r="V6" s="0" t="s">
+      <c r="V7" s="0" t="s">
         <v>71</v>
       </c>
-      <c r="W6" s="0" t="s">
-        <v>72</v>
-      </c>
-      <c r="X6" s="0" t="s">
+      <c r="W7" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="X7" s="0" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="s">
         <v>76</v>
       </c>
-      <c r="Y6" s="0" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0" t="n">
-        <v>101</v>
-      </c>
-      <c r="B7" s="0" t="s">
+      <c r="B8" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="C8" s="6" t="s">
         <v>77</v>
       </c>
-      <c r="C7" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="D7" s="6" t="s">
+      <c r="D8" s="0" t="s">
         <v>78</v>
       </c>
-      <c r="E7" s="0" t="s">
+      <c r="E8" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="F7" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="G7" s="3" t="s">
+      <c r="F8" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="G8" s="6" t="s">
         <v>81</v>
       </c>
-      <c r="H7" s="6" t="s">
+      <c r="H8" s="3" t="s">
         <v>82</v>
       </c>
-      <c r="I7" s="3" t="s">
-        <v>83</v>
-      </c>
-      <c r="J7" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="K7" s="0" t="s">
-        <v>34</v>
-      </c>
-      <c r="L7" s="0" t="n">
+      <c r="I8" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="J8" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="K8" s="0" t="n">
         <v>1199</v>
       </c>
-      <c r="M7" s="3" t="n">
+      <c r="L8" s="3" t="n">
         <v>5</v>
       </c>
-      <c r="N7" s="3"/>
-      <c r="O7" s="0" t="n">
+      <c r="M8" s="3"/>
+      <c r="N8" s="0" t="n">
         <v>4</v>
       </c>
-      <c r="P7" s="5" t="n">
+      <c r="O8" s="5" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="Q7" s="5" t="n">
+      <c r="P8" s="5" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="R7" s="5" t="n">
+      <c r="Q8" s="5" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="S7" s="5"/>
-      <c r="T7" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="U7" s="3" t="s">
+      <c r="R8" s="5"/>
+      <c r="S8" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="T8" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="U8" s="0" t="s">
         <v>70</v>
       </c>
-      <c r="V7" s="0" t="s">
+      <c r="V8" s="0" t="s">
         <v>71</v>
       </c>
-      <c r="W7" s="0" t="s">
-        <v>72</v>
-      </c>
-      <c r="X7" s="6" t="s">
-        <v>76</v>
-      </c>
-      <c r="Y7" s="0" t="s">
-        <v>84</v>
+      <c r="W8" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="X8" s="0" t="s">
+        <v>83</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="3">
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="K2:K4" type="list">
+    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="J2:J4" type="list">
       <formula1>"inr,usd,eur,gbp"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="P2:S7" type="list">
+    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="O2:R8" type="list">
       <formula1>"true,false"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="T2:T7" type="list">
+    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="S2:S8" type="list">
       <formula1>"Single,Dozen,Kilograms,Miligrams,Liters,Mililiters"</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -1343,12 +1396,12 @@
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H28" s="0" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H29" s="0" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
Priyanka kale committed changes in manual product upload
</commit_message>
<xml_diff>
--- a/admin/public/products.xlsx
+++ b/admin/public/products.xlsx
@@ -65,6 +65,27 @@
     <t xml:space="preserve">availableQuantity</t>
   </si>
   <si>
+    <t xml:space="preserve">unit</t>
+  </si>
+  <si>
+    <t xml:space="preserve">feature list</t>
+  </si>
+  <si>
+    <t xml:space="preserve">size</t>
+  </si>
+  <si>
+    <t xml:space="preserve">color</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tags</t>
+  </si>
+  <si>
+    <t xml:space="preserve">taxInclude</t>
+  </si>
+  <si>
+    <t xml:space="preserve">taxRate</t>
+  </si>
+  <si>
     <t xml:space="preserve">featured</t>
   </si>
   <si>
@@ -77,27 +98,6 @@
     <t xml:space="preserve">bestSeller</t>
   </si>
   <si>
-    <t xml:space="preserve">unit</t>
-  </si>
-  <si>
-    <t xml:space="preserve">features</t>
-  </si>
-  <si>
-    <t xml:space="preserve">size</t>
-  </si>
-  <si>
-    <t xml:space="preserve">color</t>
-  </si>
-  <si>
-    <t xml:space="preserve">tags</t>
-  </si>
-  <si>
-    <t xml:space="preserve">taxInclude</t>
-  </si>
-  <si>
-    <t xml:space="preserve">taxRate</t>
-  </si>
-  <si>
     <t xml:space="preserve">attribute Display Size  </t>
   </si>
   <si>
@@ -129,12 +129,6 @@
   </si>
   <si>
     <t xml:space="preserve">inr</t>
-  </si>
-  <si>
-    <t xml:space="preserve">no</t>
-  </si>
-  <si>
-    <t xml:space="preserve">yes</t>
   </si>
   <si>
     <t xml:space="preserve">Single</t>
@@ -152,6 +146,12 @@
   </si>
   <si>
     <t xml:space="preserve">hashtag1,hashrag2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">yes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">no</t>
   </si>
   <si>
     <t xml:space="preserve">  1.6um</t>
@@ -398,8 +398,8 @@
   <numFmts count="5">
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="#,##0"/>
-    <numFmt numFmtId="166" formatCode="&quot;TRUE&quot;;&quot;TRUE&quot;;&quot;FALSE&quot;"/>
-    <numFmt numFmtId="167" formatCode="0.0"/>
+    <numFmt numFmtId="166" formatCode="0.0"/>
+    <numFmt numFmtId="167" formatCode="&quot;TRUE&quot;;&quot;TRUE&quot;;&quot;FALSE&quot;"/>
     <numFmt numFmtId="168" formatCode="0.00%"/>
   </numFmts>
   <fonts count="17">
@@ -692,7 +692,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -808,8 +808,8 @@
   </sheetPr>
   <dimension ref="A1:AMJ8"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="T1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="X3" activeCellId="0" sqref="X3"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A17" activeCellId="0" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -827,21 +827,28 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="2" width="15.99"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="1" width="15.99"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="1" width="18.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="1" width="10.87"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="1" width="13.37"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="1" width="15.08"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="18" style="1" width="16.28"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="1" width="44.66"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="23" min="21" style="1" width="8.53"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="24" min="24" style="0" width="22.87"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="25" min="25" style="0" width="15.02"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="1" width="16.28"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="1" width="44.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="17" style="1" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="0" width="22.87"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="0" width="15.02"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="22" style="1" width="10.87"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="23" min="23" style="1" width="13.37"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="24" min="24" style="1" width="15.08"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="25" min="25" style="1" width="16.28"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="26" style="1" width="22.87"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="27" min="27" style="1" width="15.02"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1019" min="28" style="1" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="28" min="28" style="0" width="10.87"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="29" min="29" style="0" width="13.37"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="30" min="30" style="0" width="15.08"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="31" min="31" style="0" width="16.28"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="32" min="32" style="0" width="22.87"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="33" min="33" style="0" width="15.02"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1019" min="34" style="1" width="8.53"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1020" style="1" width="9.14"/>
   </cols>
   <sheetData>
-    <row r="1" s="3" customFormat="true" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" s="3" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -899,10 +906,10 @@
       <c r="S1" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="T1" s="3" t="s">
+      <c r="T1" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="U1" s="3" t="s">
+      <c r="U1" s="5" t="s">
         <v>20</v>
       </c>
       <c r="V1" s="3" t="s">
@@ -911,10 +918,10 @@
       <c r="W1" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="X1" s="5" t="s">
+      <c r="X1" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="Y1" s="5" t="s">
+      <c r="Y1" s="3" t="s">
         <v>24</v>
       </c>
       <c r="Z1" s="3" t="s">
@@ -923,6 +930,12 @@
       <c r="AA1" s="3" t="s">
         <v>26</v>
       </c>
+      <c r="AB1" s="0"/>
+      <c r="AC1" s="0"/>
+      <c r="AD1" s="0"/>
+      <c r="AE1" s="0"/>
+      <c r="AF1" s="0"/>
+      <c r="AG1" s="0"/>
       <c r="AME1" s="1"/>
       <c r="AMF1" s="1"/>
       <c r="AMG1" s="1"/>
@@ -930,7 +943,7 @@
       <c r="AMI1" s="1"/>
       <c r="AMJ1" s="1"/>
     </row>
-    <row r="2" customFormat="false" ht="123.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="107.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="6" t="s">
         <v>27</v>
       </c>
@@ -971,36 +984,36 @@
       <c r="N2" s="6" t="n">
         <v>4</v>
       </c>
-      <c r="O2" s="8"/>
-      <c r="P2" s="8" t="s">
+      <c r="O2" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="Q2" s="8" t="s">
+      <c r="P2" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="R2" s="8" t="s">
-        <v>37</v>
-      </c>
-      <c r="S2" s="9" t="s">
+      <c r="Q2" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="T2" s="6" t="s">
+      <c r="R2" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="U2" s="6" t="s">
+      <c r="S2" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="V2" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="W2" s="6" t="s">
+      <c r="T2" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="U2" s="10" t="n">
+        <v>5</v>
+      </c>
+      <c r="V2" s="9"/>
+      <c r="W2" s="9" t="s">
         <v>42</v>
       </c>
-      <c r="X2" s="8" t="s">
-        <v>37</v>
-      </c>
-      <c r="Y2" s="10" t="n">
-        <v>5</v>
+      <c r="X2" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="Y2" s="9" t="s">
+        <v>41</v>
       </c>
       <c r="Z2" s="1" t="s">
         <v>43</v>
@@ -1050,35 +1063,35 @@
       <c r="N3" s="6" t="n">
         <v>4</v>
       </c>
-      <c r="O3" s="8" t="s">
-        <v>37</v>
-      </c>
-      <c r="P3" s="8" t="s">
-        <v>37</v>
-      </c>
-      <c r="Q3" s="8" t="s">
+      <c r="O3" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="R3" s="8" t="s">
-        <v>37</v>
-      </c>
-      <c r="S3" s="6" t="s">
+      <c r="P3" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="Q3" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="T3" s="6" t="s">
-        <v>50</v>
-      </c>
-      <c r="U3" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="V3" s="1" t="s">
+      <c r="R3" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="X3" s="8" t="s">
-        <v>36</v>
-      </c>
-      <c r="Y3" s="0" t="n">
+      <c r="T3" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="U3" s="0" t="n">
         <v>5</v>
+      </c>
+      <c r="V3" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="W3" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="X3" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="Y3" s="9" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="87.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1122,35 +1135,35 @@
       <c r="N4" s="6" t="n">
         <v>4</v>
       </c>
-      <c r="O4" s="8" t="s">
+      <c r="O4" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="P4" s="8" t="s">
-        <v>37</v>
-      </c>
-      <c r="Q4" s="8" t="s">
-        <v>37</v>
-      </c>
-      <c r="R4" s="8" t="s">
-        <v>36</v>
-      </c>
-      <c r="S4" s="6" t="s">
+      <c r="P4" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="Q4" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="T4" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="U4" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="V4" s="1" t="s">
+      <c r="R4" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="X4" s="8" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="82.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="T4" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="V4" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="W4" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="X4" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="Y4" s="9" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="80.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
         <v>60</v>
       </c>
@@ -1193,35 +1206,35 @@
       <c r="N5" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="O5" s="8" t="s">
-        <v>37</v>
-      </c>
-      <c r="P5" s="8" t="s">
-        <v>37</v>
-      </c>
-      <c r="Q5" s="8" t="s">
-        <v>37</v>
-      </c>
-      <c r="R5" s="8" t="s">
-        <v>37</v>
-      </c>
-      <c r="S5" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="T5" s="6" t="s">
+      <c r="O5" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="P5" s="6" t="s">
         <v>69</v>
       </c>
-      <c r="U5" s="1" t="s">
+      <c r="Q5" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="V5" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="X5" s="8" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="82.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="R5" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="T5" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="V5" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="W5" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="X5" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="Y5" s="9" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="80.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
         <v>60</v>
       </c>
@@ -1264,32 +1277,32 @@
       <c r="N6" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="O6" s="8" t="s">
-        <v>37</v>
-      </c>
-      <c r="P6" s="8" t="s">
-        <v>37</v>
-      </c>
-      <c r="Q6" s="8" t="s">
-        <v>37</v>
-      </c>
-      <c r="R6" s="8" t="s">
-        <v>37</v>
-      </c>
-      <c r="S6" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="T6" s="6" t="s">
+      <c r="O6" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="P6" s="6" t="s">
         <v>69</v>
       </c>
-      <c r="U6" s="1" t="s">
+      <c r="Q6" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="V6" s="1" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="82.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="R6" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="V6" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="W6" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="X6" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="Y6" s="9" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="80.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
         <v>74</v>
       </c>
@@ -1332,32 +1345,32 @@
       <c r="N7" s="1" t="n">
         <v>4</v>
       </c>
-      <c r="O7" s="8" t="s">
-        <v>37</v>
-      </c>
-      <c r="P7" s="8" t="s">
-        <v>37</v>
-      </c>
-      <c r="Q7" s="8" t="s">
-        <v>37</v>
-      </c>
-      <c r="R7" s="8" t="s">
-        <v>37</v>
-      </c>
-      <c r="S7" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="T7" s="6" t="s">
+      <c r="O7" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="P7" s="6" t="s">
         <v>69</v>
       </c>
-      <c r="U7" s="6" t="s">
+      <c r="Q7" s="6" t="s">
         <v>73</v>
       </c>
-      <c r="V7" s="1" t="s">
+      <c r="R7" s="1" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="8" customFormat="false" ht="69" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="V7" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="W7" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="X7" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="Y7" s="9" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="66.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
         <v>74</v>
       </c>
@@ -1400,27 +1413,27 @@
       <c r="N8" s="1" t="n">
         <v>4</v>
       </c>
-      <c r="O8" s="8" t="s">
-        <v>37</v>
-      </c>
-      <c r="P8" s="8" t="s">
-        <v>37</v>
-      </c>
-      <c r="Q8" s="8" t="s">
-        <v>37</v>
-      </c>
-      <c r="R8" s="8" t="s">
-        <v>37</v>
-      </c>
-      <c r="S8" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="T8" s="6"/>
-      <c r="U8" s="6" t="s">
+      <c r="O8" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="P8" s="6"/>
+      <c r="Q8" s="6" t="s">
         <v>73</v>
       </c>
-      <c r="V8" s="1" t="s">
+      <c r="R8" s="1" t="s">
         <v>81</v>
+      </c>
+      <c r="V8" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="W8" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="X8" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="Y8" s="9" t="s">
+        <v>41</v>
       </c>
     </row>
   </sheetData>
@@ -1429,12 +1442,12 @@
       <formula1>"inr,usd,eur,gbp"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="S2:S8" type="list">
-      <formula1>"Single,Dozen,Kilograms,Miligrams,Liters,Mililiters"</formula1>
+    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="T2:T5 V2:Y8" type="list">
+      <formula1>"yes,no"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="O2:R8 X2:X5" type="list">
-      <formula1>"yes,no"</formula1>
+    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="O2:O8" type="list">
+      <formula1>"Single,Dozen,Kilograms,Miligrams,Liters,Mililiters"</formula1>
       <formula2>0</formula2>
     </dataValidation>
   </dataValidations>
@@ -1455,7 +1468,7 @@
   </sheetPr>
   <dimension ref="A2:O41"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A5" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A5" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="I42" activeCellId="0" sqref="I42"/>
     </sheetView>
   </sheetViews>

</xml_diff>